<commit_message>
Atualização com importação e conversão de PDF
</commit_message>
<xml_diff>
--- a/Planilhas de Teste/Pasta1.xlsx
+++ b/Planilhas de Teste/Pasta1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b2c3ffd89d078c25/Pessoal/Concept/Projeto Contabilidade/Arquivos de teste/Fontes das Macros/Planilhas de Teste/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evald\OneDrive\Pessoal\Concept\Projeto Contabilidade\Arquivos de teste\Fontes das Macros\Planilhas de Teste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{262E76C8-4632-4C48-BD44-BE96A9804B6D}" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{B6471976-DBC2-4A70-979B-C9D9CB99F0DB}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{262E76C8-4632-4C48-BD44-BE96A9804B6D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{D90F91E8-EA23-4005-A68B-71590D311926}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{A7B94E67-BC33-4111-A251-ADB55550842A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -61,8 +61,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{F5FEF495-04CC-401D-89F7-EC6574DB3F8F}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>

</xml_diff>